<commit_message>
Implemented TestNG and Modified folder structure
</commit_message>
<xml_diff>
--- a/ToolsQA_KeyWordDriven_2531/src/dataEngine/DataEngine.xlsx
+++ b/ToolsQA_KeyWordDriven_2531/src/dataEngine/DataEngine.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -286,7 +286,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -302,6 +302,10 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -644,7 +648,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,44 +659,44 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>